<commit_message>
Updated SRS, Productbacklog, and sprintbacklog
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_2/CSwap_Deliverable_2_ProductBacklog_2.xlsx
+++ b/Documents/Deliverable_2/CSwap_Deliverable_2_ProductBacklog_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ced1\Documents\GitHub\COS420_Project\Documents\Deliverable_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9A57AC-17C4-4B21-9148-2607AD3292BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F141F37-2FF4-48EF-9DA1-4BF1C009B271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1290" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7970" yWindow="2290" windowWidth="28800" windowHeight="17030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>IP</t>
-  </si>
-  <si>
     <t>As an unauthorized user I want to login to my account so that I can access my info.</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>As an authorized user I want to list furniture so that I can sell furniture I no longer need.</t>
   </si>
   <si>
-    <t>As an authorized user I want to be able to filter books by their ISBN Number.</t>
-  </si>
-  <si>
-    <t>As an authorized user I want to be able to filter all listings by key terms.</t>
-  </si>
-  <si>
     <t>As an authorized user I want to add tags to my listing so it can be found easier.</t>
   </si>
   <si>
@@ -126,7 +117,16 @@
     <t>As an authorized user I want to see how many views my listing has so that I can determine if I want to keep it up.</t>
   </si>
   <si>
-    <t>As an authorized user I want to be able to block messages from buyers that I do not want to talk to anymore.</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to be able to block messages from buyers so that I do not want to talk to anymore.</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to be able to filter books by their ISBN Number so that I can efficiently find the book.</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to be able to filter all listings by key terms so that I can narrow down my search.</t>
   </si>
 </sst>
 </file>
@@ -163,12 +163,6 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="17"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -184,6 +178,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -207,8 +208,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -236,10 +236,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,32 +257,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -542,21 +541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="71.375" customWidth="1"/>
+    <col min="1" max="1" width="10.58203125" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="4" width="26.375" customWidth="1"/>
-    <col min="5" max="5" width="27.625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.58203125" customWidth="1"/>
     <col min="6" max="6" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -589,19 +588,19 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -609,19 +608,19 @@
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -629,19 +628,19 @@
       <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>11</v>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
@@ -649,39 +648,39 @@
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="E5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="13">
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11">
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -689,19 +688,19 @@
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -709,350 +708,350 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="9">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="F10" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11">
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9">
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="11">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="11">
+      <c r="B14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9">
         <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="11">
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="9">
         <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="11">
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9">
         <v>7</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="11">
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9">
         <v>7</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="11">
+      <c r="B18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9">
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="9">
         <v>8</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="11">
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="9">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="11">
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="9">
         <v>9</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="11">
+      <c r="B22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="9">
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="11">
+      <c r="B23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="9">
         <v>10</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="11">
+      <c r="B24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="9">
         <v>11</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="11">
+      <c r="B25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="9">
         <v>11</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="11">
+        <v>16</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Product and Sprint backlog, Added Software Architecture
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_2/CSwap_Deliverable_2_ProductBacklog_2.xlsx
+++ b/Documents/Deliverable_2/CSwap_Deliverable_2_ProductBacklog_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F141F37-2FF4-48EF-9DA1-4BF1C009B271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEB97C7-7145-47AD-93B4-F6B5B935D621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7970" yWindow="2290" windowWidth="28800" windowHeight="17030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8310" yWindow="2630" windowWidth="28800" windowHeight="17030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +185,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -542,7 +546,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -632,7 +636,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -652,7 +656,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -672,7 +676,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1056,6 +1060,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>